<commit_message>
Update: Logger analyzer datetime column changed
</commit_message>
<xml_diff>
--- a/Storage/minio/storage/airflow-files/interested_tickers.xlsx
+++ b/Storage/minio/storage/airflow-files/interested_tickers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wsl\Microservices-Based-Algorithmic-Trading-System\Storage\minio\storage\airflow-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E6603-0DCC-4E64-851C-2FAC1B57618C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467F3822-B653-4E50-A86E-BDA579157AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Tickers</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>JPY_USD</t>
+  </si>
+  <si>
+    <t>AUD_USD</t>
+  </si>
+  <si>
+    <t>EUR_JPY</t>
+  </si>
+  <si>
+    <t>GBP_JPY</t>
+  </si>
+  <si>
+    <t>NZD_USD</t>
   </si>
 </sst>
 </file>
@@ -355,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -381,6 +393,26 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Dynamic Dag dictionary
</commit_message>
<xml_diff>
--- a/Storage/minio/storage/airflow-files/interested_tickers.xlsx
+++ b/Storage/minio/storage/airflow-files/interested_tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wsl\Microservices-Based-Algorithmic-Trading-System\Storage\minio\storage\airflow-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467F3822-B653-4E50-A86E-BDA579157AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D56A7-744C-4A86-8AB6-400D4A3084F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>GBP_USD</t>
   </si>
   <si>
-    <t>JPY_USD</t>
-  </si>
-  <si>
     <t>AUD_USD</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>NZD_USD</t>
+  </si>
+  <si>
+    <t>USD_JPY</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -387,7 +387,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
@@ -397,22 +397,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>